<commit_message>
lectura excel y validación de proyectos repetidos
</commit_message>
<xml_diff>
--- a/proyectos.xlsx
+++ b/proyectos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q05432593\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B28959541\Documents\laurars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E345D0-1A42-4DAB-87A7-572B429D4A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A99423-ADC5-4349-95D0-45028EF04537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3929C5C-5F02-4ABB-BB12-326D8E50090B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>AL258112</t>
   </si>
@@ -556,7 +556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,9 +564,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8167FEE-14CF-4C1D-9C2E-AED5800257E1}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -940,6 +942,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Traducción de proyectos y creación archivos
</commit_message>
<xml_diff>
--- a/proyectos.xlsx
+++ b/proyectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B28959541\Documents\laurars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A99423-ADC5-4349-95D0-45028EF04537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062B0848-190A-44A0-BD42-758C7165223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3929C5C-5F02-4ABB-BB12-326D8E50090B}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8167FEE-14CF-4C1D-9C2E-AED5800257E1}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Calculamos el presupuesto y sacamos el reporte
</commit_message>
<xml_diff>
--- a/proyectos.xlsx
+++ b/proyectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B28959541\Documents\laurars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062B0848-190A-44A0-BD42-758C7165223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F0E5B0-54F1-4048-8181-CD401D115BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3929C5C-5F02-4ABB-BB12-326D8E50090B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>AL258112</t>
   </si>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8167FEE-14CF-4C1D-9C2E-AED5800257E1}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,48 +942,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>